<commit_message>
Task 3 done for task 2
</commit_message>
<xml_diff>
--- a/Task3 Data.xlsx
+++ b/Task3 Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahrensjc1\Documents\School\Operating Systems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahrensjc1\Documents\Comp340Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -550,7 +550,7 @@
   <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,12 +663,24 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="H4" s="8">
+        <v>0.68020000000000003</v>
+      </c>
+      <c r="I4" s="9">
+        <v>3.0002</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.6573</v>
+      </c>
+      <c r="K4" s="9">
+        <v>2.0009000000000001</v>
+      </c>
+      <c r="L4" s="8">
+        <v>0.88019999999999998</v>
+      </c>
+      <c r="M4" s="9">
+        <v>5.0003000000000002</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -686,12 +698,24 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
+      <c r="H5">
+        <v>0.60009999999999997</v>
+      </c>
+      <c r="I5" s="9">
+        <v>3.0003000000000002</v>
+      </c>
+      <c r="J5">
+        <v>0.82869999999999999</v>
+      </c>
+      <c r="K5" s="9">
+        <v>3.0009000000000001</v>
+      </c>
+      <c r="L5">
+        <v>0.58020000000000005</v>
+      </c>
+      <c r="M5" s="9">
+        <v>3.0005000000000002</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -703,12 +727,24 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
+      <c r="H6">
+        <v>0.68020000000000003</v>
+      </c>
+      <c r="I6" s="9">
+        <v>3.0005999999999999</v>
+      </c>
+      <c r="J6">
+        <v>1.0002</v>
+      </c>
+      <c r="K6" s="9">
+        <v>5.0002000000000004</v>
+      </c>
+      <c r="L6">
+        <v>1.1403000000000001</v>
+      </c>
+      <c r="M6" s="9">
+        <v>7.0011000000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -720,12 +756,24 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
+      <c r="H7">
+        <v>0.48020000000000002</v>
+      </c>
+      <c r="I7" s="10">
+        <v>3.0004</v>
+      </c>
+      <c r="J7">
+        <v>0.94310000000000005</v>
+      </c>
+      <c r="K7" s="10">
+        <v>4.0011000000000001</v>
+      </c>
+      <c r="L7">
+        <v>1.2602</v>
+      </c>
+      <c r="M7" s="10">
+        <v>7.0007000000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -737,12 +785,24 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="H8">
+        <v>0.28029999999999999</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3.0007000000000001</v>
+      </c>
+      <c r="J8">
+        <v>0.60009999999999997</v>
+      </c>
+      <c r="K8" s="10">
+        <v>3.0005000000000002</v>
+      </c>
+      <c r="L8">
+        <v>1.1003000000000001</v>
+      </c>
+      <c r="M8" s="10">
+        <v>5.0003000000000002</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
@@ -772,12 +832,30 @@
         <f>MAX(B37:F86)</f>
         <v>5.0005449000000004</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
+      <c r="H9" s="18">
+        <f>AVERAGE(H4:H8)</f>
+        <v>0.54420000000000002</v>
+      </c>
+      <c r="I9" s="18">
+        <f>MAX(I4:I8)</f>
+        <v>3.0007000000000001</v>
+      </c>
+      <c r="J9" s="19">
+        <f>AVERAGE(J4:J8)</f>
+        <v>0.80588000000000015</v>
+      </c>
+      <c r="K9" s="19">
+        <f>MAX(K4:K8)</f>
+        <v>5.0002000000000004</v>
+      </c>
+      <c r="L9" s="20">
+        <f>AVERAGE(L4:L8)</f>
+        <v>0.99224000000000001</v>
+      </c>
+      <c r="M9" s="20">
+        <f>MAX(M4:M8)</f>
+        <v>7.0011000000000001</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
@@ -2598,5 +2676,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="I9:J9 K9:L9" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
now its done lol
</commit_message>
<xml_diff>
--- a/Task3 Data.xlsx
+++ b/Task3 Data.xlsx
@@ -550,7 +550,7 @@
   <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,10 +659,22 @@
         <f>MAX(B11:B35)</f>
         <v>4.0004568999999996</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="D4" s="8">
+        <f>AVERAGE(H11:H45)</f>
+        <v>1.285918785714286</v>
+      </c>
+      <c r="E4" s="8">
+        <f>MAX(H11:H45)</f>
+        <v>5.0005008999999996</v>
+      </c>
+      <c r="F4" s="8">
+        <f>AVERAGE(B37:B86)</f>
+        <v>1.2602445600000001</v>
+      </c>
+      <c r="G4" s="8">
+        <f>MAX(B37:B86)</f>
+        <v>4.0008999000000003</v>
+      </c>
       <c r="H4" s="8">
         <v>0.68020000000000003</v>
       </c>
@@ -694,10 +706,22 @@
         <f>MAX(C11:C35)</f>
         <v>5.0007258999999999</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="D5" s="8">
+        <f>AVERAGE(I11:I45)</f>
+        <v>1.5145344714285716</v>
+      </c>
+      <c r="E5" s="8">
+        <f>MAX(I11:I45)</f>
+        <v>8.0003268999999992</v>
+      </c>
+      <c r="F5" s="9">
+        <f>AVERAGE(C37:C86)</f>
+        <v>1.3402156999999997</v>
+      </c>
+      <c r="G5" s="9">
+        <f>MAX(C37:C86)</f>
+        <v>5.0002459000000004</v>
+      </c>
       <c r="H5">
         <v>0.60009999999999997</v>
       </c>
@@ -721,12 +745,30 @@
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="B6" s="9">
+        <f>AVERAGE(D11:D35)</f>
+        <v>1.2002035799999999</v>
+      </c>
+      <c r="C6" s="9">
+        <f>MAX(D11:D35)</f>
+        <v>5.0007959</v>
+      </c>
+      <c r="D6" s="8">
+        <f>AVERAGE(J11:J45)</f>
+        <v>1.7715325285714285</v>
+      </c>
+      <c r="E6" s="8">
+        <f>MAX(J11:J45)</f>
+        <v>5.0004068999999998</v>
+      </c>
+      <c r="F6" s="9">
+        <f>AVERAGE(D37:D86)</f>
+        <v>1.4801811399999993</v>
+      </c>
+      <c r="G6" s="9">
+        <f>MAX(D37:D86)</f>
+        <v>5.0005449000000004</v>
+      </c>
       <c r="H6">
         <v>0.68020000000000003</v>
       </c>
@@ -750,12 +792,30 @@
       <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="B7" s="9">
+        <f>AVERAGE(E11:E35)</f>
+        <v>1.3202097799999999</v>
+      </c>
+      <c r="C7" s="9">
+        <f>MAX(E11:E35)</f>
+        <v>4.0003168999999996</v>
+      </c>
+      <c r="D7" s="8">
+        <f>AVERAGE(K11:K45)</f>
+        <v>1.5429875857142863</v>
+      </c>
+      <c r="E7" s="8">
+        <f>MAX(K11:K45)</f>
+        <v>5.0007469000000002</v>
+      </c>
+      <c r="F7" s="9">
+        <f>AVERAGE(E37:E86)</f>
+        <v>1.26019708</v>
+      </c>
+      <c r="G7" s="9">
+        <f>MAX(E37:E86)</f>
+        <v>4.0004258999999998</v>
+      </c>
       <c r="H7">
         <v>0.48020000000000002</v>
       </c>
@@ -779,12 +839,30 @@
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="B8" s="10">
+        <f>AVERAGE(F11:F35)</f>
+        <v>1.4402141800000001</v>
+      </c>
+      <c r="C8" s="10">
+        <f>MAX(F11:F35)</f>
+        <v>6.0005008999999996</v>
+      </c>
+      <c r="D8" s="8">
+        <f>AVERAGE(L11:L45)</f>
+        <v>1.2287079857142857</v>
+      </c>
+      <c r="E8" s="8">
+        <f>MAX(L11:L45)</f>
+        <v>6.0004308999999996</v>
+      </c>
+      <c r="F8" s="10">
+        <f>AVERAGE(F37:F86)</f>
+        <v>1.2601339399999996</v>
+      </c>
+      <c r="G8" s="10">
+        <f>MAX(F37:F86)</f>
+        <v>5.0002918999999997</v>
+      </c>
       <c r="H8">
         <v>0.28029999999999999</v>
       </c>

</xml_diff>